<commit_message>
Add refresh button for template packages
</commit_message>
<xml_diff>
--- a/template/Test/config.xlsx
+++ b/template/Test/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philbertloekman/Documents/GitHub/docufill/template/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B45FD1D-5C48-3542-95F9-D925ABF5F971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A7FAEE-C917-AD4B-BC1C-BEEFA7C1747B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15120" yWindow="760" windowWidth="15120" windowHeight="17300" xr2:uid="{6472B95A-469B-3646-8BE9-5A1E8E6DAAC4}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="A5" sqref="A5:C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>